<commit_message>
Added 1A resettable fuse to 12V power
</commit_message>
<xml_diff>
--- a/pcb/PaprControlPCB/PCBA Manufacturing Files/PaprControl v0.3 BOM JLCPCB.xlsx
+++ b/pcb/PaprControlPCB/PCBA Manufacturing Files/PaprControl v0.3 BOM JLCPCB.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23530"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pc\OneDrive\GitHub\PAPRA-PCB\pcb\PCB v0.20\PCBA Manufacturing Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a412b16b128866ae/GitHub/PAPRA-PCB/pcb/PaprControlPCB/PCBA Manufacturing Files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91E44D96-F9E5-4592-81F8-011BD091A72B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="7" documentId="13_ncr:1_{91E44D96-F9E5-4592-81F8-011BD091A72B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{8D2CFF13-B2E0-468D-9570-0D64A9701327}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15945" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14002" yWindow="727" windowWidth="14798" windowHeight="12496" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="54">
   <si>
     <t>Comment</t>
   </si>
@@ -216,6 +216,12 @@
   </si>
   <si>
     <t>C481364</t>
+  </si>
+  <si>
+    <t>F1</t>
+  </si>
+  <si>
+    <t>C70081</t>
   </si>
 </sst>
 </file>
@@ -596,10 +602,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.9296875" defaultRowHeight="14.25"/>
@@ -681,139 +687,151 @@
       </c>
     </row>
     <row r="6" spans="1:4">
-      <c r="A6" s="3" t="s">
-        <v>25</v>
-      </c>
+      <c r="A6" s="3"/>
       <c r="B6" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>13</v>
+        <v>52</v>
+      </c>
+      <c r="C6" s="3">
+        <v>1206</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>35</v>
+        <v>53</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>6</v>
+        <v>44</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>45</v>
+        <v>6</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>20</v>
+        <v>45</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>15</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>15</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>16</v>
+        <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:4">
-      <c r="A11" s="3">
-        <v>330</v>
+      <c r="A11" s="3" t="s">
+        <v>29</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>15</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:4">
-      <c r="A12" s="3" t="s">
-        <v>30</v>
+      <c r="A12" s="3">
+        <v>330</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>15</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>39</v>
+        <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>15</v>
       </c>
       <c r="D13" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D14" s="2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
-      <c r="A14" s="4" t="s">
+    <row r="15" spans="1:4">
+      <c r="A15" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B15" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C15" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="D15" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
-      <c r="B15" s="3" t="s">
+    <row r="16" spans="1:4">
+      <c r="B16" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C16" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="D16" s="2" t="s">
         <v>51</v>
       </c>
     </row>

</xml_diff>